<commit_message>
finnnished reading in sheets
</commit_message>
<xml_diff>
--- a/UI-path/excel table/Connected Office Test Data (1).xlsx
+++ b/UI-path/excel table/Connected Office Test Data (1).xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jacqui.Muller\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mega\OneDrive\Documents\3 de jaar\323\project 3\CMPG-323-Overview--Project-4-34329625\UI-path\excel table\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCAB8EEF-425E-42A8-A7F1-FF25847C778D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Device" sheetId="1" r:id="rId1"/>
@@ -33,8 +32,8 @@
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
-  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" name="MOCK_DATA" type="6" refreshedVersion="6" background="1" saveData="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <connection id="1" name="MOCK_DATA" type="6" refreshedVersion="6" background="1" saveData="1">
     <textPr codePage="850" sourceFile="D:\Downloads\MOCK_DATA.csv" thousands=" " comma="1">
       <textFields count="5">
         <textField/>
@@ -45,7 +44,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="2" xr16:uid="{00000000-0015-0000-FFFF-FFFF01000000}" name="MOCK_DATA(1)" type="6" refreshedVersion="6" background="1" saveData="1">
+  <connection id="2" name="MOCK_DATA(1)" type="6" refreshedVersion="6" background="1" saveData="1">
     <textPr codePage="850" sourceFile="D:\Downloads\MOCK_DATA(1).csv" thousands=" " tab="0" comma="1">
       <textFields count="2">
         <textField/>
@@ -53,7 +52,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="3" xr16:uid="{00000000-0015-0000-FFFF-FFFF02000000}" name="MOCK_DATA(2)" type="6" refreshedVersion="6" background="1" saveData="1">
+  <connection id="3" name="MOCK_DATA(2)" type="6" refreshedVersion="6" background="1" saveData="1">
     <textPr codePage="850" sourceFile="D:\Downloads\MOCK_DATA(2).csv" thousands=" " comma="1">
       <textFields count="2">
         <textField/>
@@ -295,7 +294,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -376,15 +375,15 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="MOCK_DATA" connectionId="1" xr16:uid="{00000000-0016-0000-0000-000000000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="MOCK_DATA" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="MOCK_DATA(1)" connectionId="2" xr16:uid="{00000000-0016-0000-0100-000001000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="MOCK_DATA(1)" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="MOCK_DATA(2)" connectionId="3" xr16:uid="{00000000-0016-0000-0200-000002000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="MOCK_DATA(2)" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -683,23 +682,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>47</v>
       </c>
@@ -719,7 +718,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>48</v>
       </c>
@@ -739,7 +738,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>49</v>
       </c>
@@ -759,7 +758,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>50</v>
       </c>
@@ -779,7 +778,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>51</v>
       </c>
@@ -799,7 +798,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>52</v>
       </c>
@@ -819,7 +818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>53</v>
       </c>
@@ -839,7 +838,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>54</v>
       </c>
@@ -859,7 +858,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>55</v>
       </c>
@@ -879,7 +878,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>56</v>
       </c>
@@ -907,20 +906,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="46.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="46.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>47</v>
       </c>
@@ -931,7 +930,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>57</v>
       </c>
@@ -942,7 +941,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>58</v>
       </c>
@@ -953,7 +952,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>59</v>
       </c>
@@ -964,7 +963,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>60</v>
       </c>
@@ -975,7 +974,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>61</v>
       </c>
@@ -986,7 +985,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>62</v>
       </c>
@@ -997,7 +996,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>63</v>
       </c>
@@ -1008,7 +1007,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>64</v>
       </c>
@@ -1019,7 +1018,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>65</v>
       </c>
@@ -1037,21 +1036,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="41.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="53.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="53.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>47</v>
       </c>
@@ -1062,7 +1061,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>66</v>
       </c>
@@ -1073,7 +1072,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>67</v>
       </c>
@@ -1084,7 +1083,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>68</v>
       </c>
@@ -1095,7 +1094,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>69</v>
       </c>
@@ -1106,7 +1105,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>70</v>
       </c>
@@ -1124,22 +1123,22 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{243FE4D3-E987-44A9-BA20-E766DD09E091}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>47</v>
       </c>
@@ -1156,7 +1155,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>57</v>
       </c>
@@ -1173,7 +1172,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>58</v>
       </c>
@@ -1190,7 +1189,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>59</v>
       </c>
@@ -1207,7 +1206,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>60</v>
       </c>
@@ -1224,7 +1223,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>61</v>
       </c>
@@ -1241,7 +1240,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>62</v>
       </c>
@@ -1258,7 +1257,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>63</v>
       </c>
@@ -1275,7 +1274,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>64</v>
       </c>
@@ -1292,7 +1291,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>65</v>
       </c>
@@ -1309,7 +1308,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>66</v>
       </c>
@@ -1326,7 +1325,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>67</v>
       </c>
@@ -1343,7 +1342,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>68</v>
       </c>
@@ -1360,7 +1359,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>69</v>
       </c>
@@ -1377,7 +1376,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>70</v>
       </c>
@@ -1394,7 +1393,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>48</v>
       </c>
@@ -1411,7 +1410,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>49</v>
       </c>
@@ -1428,7 +1427,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>50</v>
       </c>
@@ -1445,7 +1444,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>51</v>
       </c>
@@ -1462,7 +1461,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>52</v>
       </c>
@@ -1479,7 +1478,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>53</v>
       </c>
@@ -1496,7 +1495,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>54</v>
       </c>
@@ -1513,7 +1512,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>55</v>
       </c>
@@ -1530,7 +1529,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>56</v>
       </c>

</xml_diff>